<commit_message>
serverStatusCoC en checker toegevoegd
</commit_message>
<xml_diff>
--- a/clanoverview_logs/generated_reports/2017-12-20_clanlog.xlsx
+++ b/clanoverview_logs/generated_reports/2017-12-20_clanlog.xlsx
@@ -116,6 +116,12 @@
     <t>#QLV8Q0C0</t>
   </si>
   <si>
+    <t>tomtoch</t>
+  </si>
+  <si>
+    <t>#8299JUJY</t>
+  </si>
+  <si>
     <t>GJS</t>
   </si>
   <si>
@@ -128,12 +134,6 @@
     <t>#QU0VGY9</t>
   </si>
   <si>
-    <t>tomtoch</t>
-  </si>
-  <si>
-    <t>#8299JUJY</t>
-  </si>
-  <si>
     <t>leeuw</t>
   </si>
   <si>
@@ -152,24 +152,30 @@
     <t>#YVYU9Y8R</t>
   </si>
   <si>
+    <t>xavier</t>
+  </si>
+  <si>
+    <t>#8P88LUCQ</t>
+  </si>
+  <si>
     <t>rommensje</t>
   </si>
   <si>
     <t>#9Y0URQUL</t>
   </si>
   <si>
-    <t>xavier</t>
-  </si>
-  <si>
-    <t>#8P88LUCQ</t>
-  </si>
-  <si>
     <t>duke en wesj</t>
   </si>
   <si>
     <t>#P0PV2CJY</t>
   </si>
   <si>
+    <t>THICK GIRLS</t>
+  </si>
+  <si>
+    <t>#8U09PR0V</t>
+  </si>
+  <si>
     <t>Bastos</t>
   </si>
   <si>
@@ -179,12 +185,6 @@
     <t>member</t>
   </si>
   <si>
-    <t>THICK GIRLS</t>
-  </si>
-  <si>
-    <t>#8U09PR0V</t>
-  </si>
-  <si>
     <t>(j)de tik(j)</t>
   </si>
   <si>
@@ -209,34 +209,34 @@
     <t>#828YUV9J</t>
   </si>
   <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>#8LV09JG9</t>
+  </si>
+  <si>
     <t>elandro</t>
   </si>
   <si>
     <t>#22GU992L</t>
   </si>
   <si>
-    <t>peter</t>
-  </si>
-  <si>
-    <t>#8LV09JG9</t>
+    <t>mauzer99</t>
+  </si>
+  <si>
+    <t>#P8VQ09QQ</t>
+  </si>
+  <si>
+    <t>kevintjuh93</t>
+  </si>
+  <si>
+    <t>#YG0URYGQ</t>
   </si>
   <si>
     <t>axes</t>
   </si>
   <si>
     <t>#2JVRYC22</t>
-  </si>
-  <si>
-    <t>mauzer99</t>
-  </si>
-  <si>
-    <t>#P8VQ09QQ</t>
-  </si>
-  <si>
-    <t>kevintjuh93</t>
-  </si>
-  <si>
-    <t>#YG0URYGQ</t>
   </si>
   <si>
     <t>wiski</t>
@@ -445,13 +445,13 @@
         <v>11</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>5313.0</v>
+        <v>5345.0</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>5473.0</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="3">
@@ -468,19 +468,19 @@
         <v>197.0</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>5550.0</v>
+        <v>5548.0</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>9811.0</v>
+        <v>10067.0</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>4877.0</v>
+        <v>4914.0</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>2.01</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="4">
@@ -497,19 +497,19 @@
         <v>179.0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>5355.0</v>
+        <v>5380.0</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>1353.0</v>
+        <v>1392.0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>1313.0</v>
+        <v>1387.0</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>1.03</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -584,7 +584,7 @@
         <v>169.0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>5116.0</v>
+        <v>5119.0</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
@@ -613,7 +613,7 @@
         <v>184.0</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>5059.0</v>
+        <v>5043.0</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -622,10 +622,10 @@
         <v>1889.0</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>1307.0</v>
+        <v>1344.0</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>1.45</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="9">
@@ -642,7 +642,7 @@
         <v>189.0</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>4959.0</v>
+        <v>4955.0</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>14</v>
@@ -671,19 +671,19 @@
         <v>210.0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>4927.0</v>
+        <v>4933.0</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>5340.0</v>
+        <v>5451.0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>2714.0</v>
+        <v>2751.0</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>1.97</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="11">
@@ -700,19 +700,19 @@
         <v>159.0</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>4906.0</v>
+        <v>4911.0</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>687.0</v>
+        <v>759.0</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>953.0</v>
+        <v>990.0</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="12">
@@ -729,7 +729,7 @@
         <v>172.0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>4833.0</v>
+        <v>4836.0</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -755,22 +755,22 @@
         <v>35</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>161.0</v>
+        <v>179.0</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>4826.0</v>
+        <v>4825.0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>3204.0</v>
+        <v>1138.0</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>3452.0</v>
+        <v>1661.0</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>0.93</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="14">
@@ -784,22 +784,22 @@
         <v>37</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>175.0</v>
+        <v>161.0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>4800.0</v>
+        <v>4816.0</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>1458.0</v>
+        <v>3305.0</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>2048.0</v>
+        <v>3526.0</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.71</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="15">
@@ -813,22 +813,22 @@
         <v>39</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>179.0</v>
+        <v>175.0</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>4799.0</v>
+        <v>4800.0</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>1096.0</v>
+        <v>1488.0</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>1476.0</v>
+        <v>2120.0</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16">
@@ -845,19 +845,19 @@
         <v>174.0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>4792.0</v>
+        <v>4795.0</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>3543.0</v>
+        <v>3704.0</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>5629.0</v>
+        <v>5666.0</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="17">
@@ -903,7 +903,7 @@
         <v>179.0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>4716.0</v>
+        <v>4712.0</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -929,22 +929,22 @@
         <v>47</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>191.0</v>
+        <v>181.0</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>4610.0</v>
+        <v>4614.0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>1496.0</v>
+        <v>6697.0</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>1263.0</v>
+        <v>6746.0</v>
       </c>
       <c r="I19" s="3" t="n">
-        <v>1.18</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="20">
@@ -958,22 +958,22 @@
         <v>49</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>181.0</v>
+        <v>191.0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4605.0</v>
+        <v>4610.0</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>6690.0</v>
+        <v>1496.0</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>6598.0</v>
+        <v>1263.0</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>1.01</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="21">
@@ -990,19 +990,19 @@
         <v>211.0</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>4585.0</v>
+        <v>4609.0</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="3" t="n">
-        <v>6651.0</v>
+        <v>6784.0</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>4042.0</v>
+        <v>4077.0</v>
       </c>
       <c r="I21" s="3" t="n">
-        <v>1.65</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="22">
@@ -1016,22 +1016,22 @@
         <v>53</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>172.0</v>
+        <v>183.0</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>4568.0</v>
+        <v>4571.0</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>37.0</v>
+        <v>1401.0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0.0</v>
+        <v>1353.0</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>0.0</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="23">
@@ -1039,28 +1039,28 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="3" t="n">
+        <v>172.0</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>4568.0</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="3" t="n">
-        <v>183.0</v>
-      </c>
-      <c r="E23" s="3" t="n">
-        <v>4566.0</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="G23" s="3" t="n">
-        <v>1401.0</v>
+        <v>37.0</v>
       </c>
       <c r="H23" s="3" t="n">
-        <v>1316.0</v>
+        <v>0.0</v>
       </c>
       <c r="I23" s="3" t="n">
-        <v>1.06</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="24">
@@ -1077,7 +1077,7 @@
         <v>178.0</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>4554.0</v>
+        <v>4556.0</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -1086,7 +1086,7 @@
         <v>612.0</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>1550.0</v>
+        <v>1587.0</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>0.39</v>
@@ -1141,10 +1141,10 @@
         <v>14</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>1224.0</v>
+        <v>1261.0</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>2103.0</v>
+        <v>2175.0</v>
       </c>
       <c r="I26" s="2" t="n">
         <v>0.58</v>
@@ -1167,7 +1167,7 @@
         <v>4395.0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G27" s="3" t="n">
         <v>1063.0</v>
@@ -1190,22 +1190,22 @@
         <v>66</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>175.0</v>
+        <v>159.0</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>4286.0</v>
+        <v>4316.0</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>2988.0</v>
+        <v>2167.0</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>3721.0</v>
+        <v>3173.0</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="29">
@@ -1219,22 +1219,22 @@
         <v>68</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>159.0</v>
+        <v>175.0</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>4268.0</v>
+        <v>4285.0</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G29" s="3" t="n">
-        <v>2100.0</v>
+        <v>2989.0</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>3094.0</v>
+        <v>3791.0</v>
       </c>
       <c r="I29" s="3" t="n">
-        <v>0.68</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="30">
@@ -1248,22 +1248,22 @@
         <v>70</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>168.0</v>
+        <v>172.0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4125.0</v>
+        <v>4065.0</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>3050.0</v>
+        <v>31.0</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>3717.0</v>
+        <v>183.0</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>0.82</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="31">
@@ -1277,22 +1277,22 @@
         <v>72</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>172.0</v>
+        <v>146.0</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>4065.0</v>
+        <v>4031.0</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G31" s="3" t="n">
-        <v>31.0</v>
+        <v>424.0</v>
       </c>
       <c r="H31" s="3" t="n">
-        <v>183.0</v>
+        <v>406.0</v>
       </c>
       <c r="I31" s="3" t="n">
-        <v>0.17</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="32">
@@ -1306,22 +1306,22 @@
         <v>74</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>146.0</v>
+        <v>168.0</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>4027.0</v>
+        <v>4030.0</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>419.0</v>
+        <v>3050.0</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>369.0</v>
+        <v>3789.0</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>1.14</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="33">
@@ -1338,7 +1338,7 @@
         <v>155.0</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>3796.0</v>
+        <v>3788.0</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>23</v>
@@ -1370,7 +1370,7 @@
         <v>3609.0</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>190.0</v>
@@ -1379,7 +1379,7 @@
         <v>0.0</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>0.0</v>
+        <v>190.0</v>
       </c>
     </row>
     <row r="35">
@@ -1396,19 +1396,19 @@
         <v>170.0</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>3604.0</v>
+        <v>3591.0</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="3" t="n">
-        <v>7116.0</v>
+        <v>7185.0</v>
       </c>
       <c r="H35" s="3" t="n">
-        <v>5626.0</v>
+        <v>5661.0</v>
       </c>
       <c r="I35" s="3" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="36">
@@ -1425,10 +1425,10 @@
         <v>131.0</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>3525.0</v>
+        <v>3513.0</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>1401.0</v>
@@ -1454,7 +1454,7 @@
         <v>214.0</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>3453.0</v>
+        <v>3483.0</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>23</v>
@@ -1483,19 +1483,19 @@
         <v>156.0</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>3448.0</v>
+        <v>3445.0</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>586.0</v>
+        <v>638.0</v>
       </c>
       <c r="H38" s="2" t="n">
         <v>389.0</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>1.51</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="39">
@@ -1512,7 +1512,7 @@
         <v>151.0</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>3446.0</v>
+        <v>3424.0</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>14</v>
@@ -1541,7 +1541,7 @@
         <v>123.0</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>3365.0</v>
+        <v>3371.0</v>
       </c>
       <c r="F40" t="s">
         <v>23</v>
@@ -1570,19 +1570,19 @@
         <v>165.0</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>3079.0</v>
+        <v>3124.0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G41" s="3" t="n">
-        <v>1230.0</v>
+        <v>1306.0</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>835.0</v>
+        <v>914.0</v>
       </c>
       <c r="I41" s="3" t="n">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="42">
@@ -1599,7 +1599,7 @@
         <v>112.0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>2482.0</v>
+        <v>2478.0</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -1628,10 +1628,10 @@
         <v>69.0</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>1310.0</v>
+        <v>1330.0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G43" s="3" t="n">
         <v>0.0</v>
@@ -1646,7 +1646,7 @@
   </sheetData>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.25" right="0.25" top="0.5"/>
   <headerFooter>
-    <oddFooter>&amp;LClanoverzicht&amp;R20/12/2017 10:36</oddFooter>
+    <oddFooter>&amp;LClanoverzicht&amp;R20/12/2017 16:37</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>